<commit_message>
Updated to MEPOS V0.5
-updated pinout so pin names matched schematic.
-added paste holes for alignment
</commit_message>
<xml_diff>
--- a/Header Pinout.xlsx
+++ b/Header Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomfr\Desktop\Repos\1. MEPOS\MEPOS_Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomfr\Desktop\Repos\Fried Electronics\MEPOS-Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FBE720-F9D0-4BBF-B0D5-720160A51750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8EC8E7-B676-4B44-89F0-F818BEDD3800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{8DBED372-6BC2-4B37-9514-78375B0F2E34}"/>
   </bookViews>
@@ -330,40 +330,40 @@
     <t>TX2</t>
   </si>
   <si>
-    <t>~GPIO2</t>
-  </si>
-  <si>
-    <t>~GPIO1</t>
-  </si>
-  <si>
-    <t>~GPIO4</t>
-  </si>
-  <si>
-    <t>~GPIO3</t>
-  </si>
-  <si>
-    <t>~GPIO16</t>
-  </si>
-  <si>
-    <t>~GPIO18</t>
-  </si>
-  <si>
-    <t>~GPIO15</t>
-  </si>
-  <si>
-    <t>~GPIO17</t>
-  </si>
-  <si>
-    <t>(~)GPIOx</t>
-  </si>
-  <si>
     <t>General Purpose IO (Timer/PWM)</t>
   </si>
   <si>
-    <t>~GPIO20</t>
-  </si>
-  <si>
-    <t>~GPIO19</t>
+    <t>GPIO1~</t>
+  </si>
+  <si>
+    <t>GPIO3~</t>
+  </si>
+  <si>
+    <t>GPIO2~</t>
+  </si>
+  <si>
+    <t>GPIO4~</t>
+  </si>
+  <si>
+    <t>GPIO16~</t>
+  </si>
+  <si>
+    <t>GPIO15~</t>
+  </si>
+  <si>
+    <t>GPIO17~</t>
+  </si>
+  <si>
+    <t>GPIO19~</t>
+  </si>
+  <si>
+    <t>GPIO18~</t>
+  </si>
+  <si>
+    <t>GPIO20~</t>
+  </si>
+  <si>
+    <t>GPIOx(~)</t>
   </si>
 </sst>
 </file>
@@ -879,7 +879,7 @@
   <dimension ref="B2:O35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1005,10 +1005,10 @@
         <v>6</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
@@ -1393,7 +1393,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="17" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C19" s="3">
         <v>32</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C20" s="3">
         <v>34</v>
@@ -1428,7 +1428,7 @@
         <v>33</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>28</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="3">
         <v>46</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C27" s="3">
         <v>48</v>
@@ -1604,7 +1604,7 @@
         <v>49</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="6"/>

</xml_diff>